<commit_message>
add battle end add exp & sell equips
</commit_message>
<xml_diff>
--- a/Data/FoodDefine.xlsx
+++ b/Data/FoodDefine.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>ID</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>property4.floatFactor</t>
-  </si>
-  <si>
-    <t>priceFloatFactor</t>
   </si>
   <si>
     <t>胡萝卜须</t>
@@ -1252,10 +1249,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C12" sqref="A1:C12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -1272,10 +1269,9 @@
     <col min="12" max="12" width="13.3076923076923" customWidth="1"/>
     <col min="13" max="13" width="16.2692307692308" customWidth="1"/>
     <col min="14" max="14" width="20.2115384615385" customWidth="1"/>
-    <col min="15" max="15" width="16.2692307692308" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1318,16 +1314,13 @@
       <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:11">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1">
         <v>18</v>
@@ -1356,16 +1349,13 @@
       <c r="K2">
         <v>2</v>
       </c>
-      <c r="O2">
-        <v>20</v>
-      </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:11">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1">
         <v>18</v>
@@ -1394,16 +1384,13 @@
       <c r="K3">
         <v>2</v>
       </c>
-      <c r="O3">
-        <v>20</v>
-      </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:11">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1">
         <v>18</v>
@@ -1432,16 +1419,13 @@
       <c r="K4">
         <v>1</v>
       </c>
-      <c r="O4">
-        <v>20</v>
-      </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:11">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1">
         <v>18</v>
@@ -1470,16 +1454,13 @@
       <c r="K5">
         <v>2</v>
       </c>
-      <c r="O5">
-        <v>20</v>
-      </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:11">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1">
         <v>18</v>
@@ -1508,16 +1489,13 @@
       <c r="K6">
         <v>1</v>
       </c>
-      <c r="O6">
-        <v>20</v>
-      </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:14">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1">
         <v>18</v>
@@ -1555,16 +1533,13 @@
       <c r="N7">
         <v>3</v>
       </c>
-      <c r="O7">
-        <v>40</v>
-      </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:14">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1">
         <v>18</v>
@@ -1602,16 +1577,13 @@
       <c r="N8">
         <v>2</v>
       </c>
-      <c r="O8">
-        <v>20</v>
-      </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:14">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1">
         <v>18</v>
@@ -1649,16 +1621,13 @@
       <c r="N9">
         <v>2</v>
       </c>
-      <c r="O9">
-        <v>10</v>
-      </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:8">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1">
         <v>18</v>
@@ -1678,16 +1647,13 @@
       <c r="H10">
         <v>3</v>
       </c>
-      <c r="O10">
-        <v>10</v>
-      </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:8">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="1">
         <v>18</v>
@@ -1707,16 +1673,13 @@
       <c r="H11">
         <v>5</v>
       </c>
-      <c r="O11">
-        <v>10</v>
-      </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:6">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="1">
         <v>18</v>
@@ -1728,9 +1691,6 @@
         <v>0</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="O12">
-        <v>10</v>
-      </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="1"/>

</xml_diff>